<commit_message>
Inicio consulta de costo V!
</commit_message>
<xml_diff>
--- a/APP_PERSONAS_XML/src/test/resources/datadriven/inversionvirtual/Trn_0322ConsultarTasas.xlsx
+++ b/APP_PERSONAS_XML/src/test/resources/datadriven/inversionvirtual/Trn_0322ConsultarTasas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AUTOMATIZACION JAVA\PROYECTOS GRADLE\PROYECTOS XML\PITTS_CanalesVirtuales_XML_TEST\src\test\resources\datadriven\virtualinvestment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AUTOMATIZACION JAVA\PROYECTOS GRADLE\PROYECTOS NUEVA APP\AW1059001_NuevaAPPSucursalVirtualPersonas_Test\APP_PERSONAS_XML\src\test\resources\datadriven\inversionvirtual\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
   <si>
     <t>orientacion</t>
   </si>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t>TRANSACCION EXITOSA</t>
+  </si>
+  <si>
+    <t>030</t>
+  </si>
+  <si>
+    <t>ERROR</t>
   </si>
 </sst>
 </file>
@@ -539,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -637,16 +643,16 @@
         <v>33</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>37</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:10">

</xml_diff>